<commit_message>
more test cases for activity api
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity_Productivity.xlsx
+++ b/src/test/resources/data/Activity_Productivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1AE002-90FC-47BC-B52C-4E35FF43FEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C142F1D-B310-485C-83AA-D48E0CA263B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1330" yWindow="290" windowWidth="17490" windowHeight="9180" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="40" yWindow="440" windowWidth="19160" windowHeight="9760" activeTab="2" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="44">
   <si>
     <t>TCID</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>400error.json</t>
+  </si>
+  <si>
+    <t>getUserSessionsSchema.json</t>
+  </si>
+  <si>
+    <t>getSimultaniousActivitySchema.json</t>
   </si>
 </sst>
 </file>
@@ -543,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7E84D1-294A-4626-81FA-9856648E2C09}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -718,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B88D30-C8DE-42A0-A9E2-8B6287FAD006}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -838,10 +844,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1505332-9685-449B-8C4A-AB02E3790084}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -852,10 +858,9 @@
     <col min="6" max="6" width="67.08984375" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="8" width="25.81640625" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -880,11 +885,8 @@
       <c r="H1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -906,12 +908,11 @@
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -931,9 +932,8 @@
       <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>10</v>
+      <c r="H3" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1025,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3388F2-1909-45A3-81C6-E34A543E1DC2}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1090,7 +1090,9 @@
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="I2" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
fixed the schema validator
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity_Productivity.xlsx
+++ b/src/test/resources/data/Activity_Productivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47822552-014F-41BF-B0AC-AECE2F627E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3757B5-C35B-4A00-AD55-5EBA70DADCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35415" yWindow="-10560" windowWidth="19185" windowHeight="10200" firstSheet="3" activeTab="4" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="18615" yWindow="-19950" windowWidth="19740" windowHeight="14880" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="48">
   <si>
     <t>TCID</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>GET_user_summary.json</t>
+  </si>
+  <si>
+    <t>GET_last_login.json</t>
   </si>
 </sst>
 </file>
@@ -572,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7E84D1-294A-4626-81FA-9856648E2C09}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -748,7 +751,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -812,7 +815,9 @@
       <c r="G2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="I2" s="6" t="s">
         <v>39</v>
       </c>
@@ -872,7 +877,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1087,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C3772B-6738-4612-BB2C-6B6DC76D6E13}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
more test cases completed
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity_Productivity.xlsx
+++ b/src/test/resources/data/Activity_Productivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3757B5-C35B-4A00-AD55-5EBA70DADCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB68698E-EA5D-4D58-9BF0-1BAB5B75F7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18615" yWindow="-19950" windowWidth="19740" windowHeight="14880" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="10" yWindow="600" windowWidth="19190" windowHeight="10200" firstSheet="3" activeTab="5" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="80">
   <si>
     <t>TCID</t>
   </si>
@@ -184,6 +184,102 @@
   </si>
   <si>
     <t>GET_last_login.json</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Get random equipmentId</t>
+  </si>
+  <si>
+    <t>Get User Activity By equipmentId</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Get User activity by locationId</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y </t>
+  </si>
+  <si>
+    <t>Get User activity by equipmentTypeId</t>
+  </si>
+  <si>
+    <t>Get random equipmentTypeId</t>
+  </si>
+  <si>
+    <t>Get random locationId</t>
+  </si>
+  <si>
+    <t>/activity/v1/users?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1&amp;equipmentId={equipmentId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1&amp;locationId={locationId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1&amp;equipmentTypeId={equipmentTypeId}</t>
+  </si>
+  <si>
+    <t>Get Last login with invalid userId and valid equipmentId</t>
+  </si>
+  <si>
+    <t>Get Last login with valid userId and invalid equipmentId</t>
+  </si>
+  <si>
+    <t>Get last login, filter by equipmentId</t>
+  </si>
+  <si>
+    <t>Get last login, filter by equipmentTypeId</t>
+  </si>
+  <si>
+    <t>Get last login, filter by locationId</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/last-logins?equipmentId={equipmentId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/last-logins?locationId={locationId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/last-logins?equipmentTypeId={equipmentTypeId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}0/last-logins?equipmentTypeId={equipmentTypeId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/last-logins?equipmentTypeId={equipmentTypeId}0</t>
+  </si>
+  <si>
+    <t>Get User Activity with startTimeStamp and endTimeStamp queries</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/last-logins?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/last-logins?startTimestamp=2020-5-1</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/last-logins?pageSize=1</t>
+  </si>
+  <si>
+    <t>Get userId, equipment, equipmentTypeId, and locationId</t>
+  </si>
+  <si>
+    <t>Get Simultaneous User Activity for invalid User</t>
+  </si>
+  <si>
+    <t>Get user Summary For invalidUser</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/a416e744-c66f-48b1-af78-055aa30aa982/summary</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/a416e744-c66f-48b1-af78-055aa30aa982/simultaneous-logins?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1</t>
   </si>
 </sst>
 </file>
@@ -212,7 +308,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,12 +318,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF7C80"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -244,15 +334,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -573,17 +666,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7E84D1-294A-4626-81FA-9856648E2C09}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="8.7265625" style="1"/>
     <col min="3" max="3" width="45" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.54296875" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.81640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="50.26953125" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.36328125" style="1" customWidth="1"/>
@@ -739,6 +832,84 @@
         <v>40</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -748,17 +919,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B88D30-C8DE-42A0-A9E2-8B6287FAD006}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="30.81640625" customWidth="1"/>
+    <col min="3" max="3" width="55.90625" customWidth="1"/>
     <col min="4" max="4" width="43.90625" customWidth="1"/>
-    <col min="6" max="6" width="52.6328125" customWidth="1"/>
+    <col min="6" max="6" width="68.1796875" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="8" width="25.81640625" customWidth="1"/>
     <col min="9" max="9" width="26.1796875" customWidth="1"/>
@@ -793,32 +964,32 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
+    <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -848,23 +1019,210 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5">
+        <v>200</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6">
+        <v>200</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7">
+        <v>400</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8">
+        <v>400</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9">
+        <v>200</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10">
+        <v>200</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -876,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3388F2-1909-45A3-81C6-E34A543E1DC2}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -993,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1505332-9685-449B-8C4A-AB02E3790084}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1090,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C3772B-6738-4612-BB2C-6B6DC76D6E13}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1159,6 +1517,29 @@
         <v>45</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3">
+        <v>400</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1168,13 +1549,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086B76B2-2B82-421F-92E2-E6E040E4DE28}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="21.54296875" customWidth="1"/>
+    <col min="3" max="3" width="36.453125" customWidth="1"/>
     <col min="4" max="4" width="43.90625" customWidth="1"/>
     <col min="6" max="6" width="36.08984375" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
@@ -1235,14 +1616,28 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>

</xml_diff>

<commit_message>
Completed autmation for Activity - productivity
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity_Productivity.xlsx
+++ b/src/test/resources/data/Activity_Productivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB68698E-EA5D-4D58-9BF0-1BAB5B75F7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095D566B-BAF7-4323-BFCD-BC43DAB8913E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="600" windowWidth="19190" windowHeight="10200" firstSheet="3" activeTab="5" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="990" yWindow="0" windowWidth="18510" windowHeight="10110" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="115">
   <si>
     <t>TCID</t>
   </si>
@@ -159,9 +159,6 @@
     <t>400error.json</t>
   </si>
   <si>
-    <t>The response does not return startSessionTimestamp field as expected by the swagger doc</t>
-  </si>
-  <si>
     <t>GET_activity_v1_users.json</t>
   </si>
   <si>
@@ -249,12 +246,6 @@
     <t>/activity/v1/users/{userId}/last-logins?equipmentTypeId={equipmentTypeId}</t>
   </si>
   <si>
-    <t>/activity/v1/users/{userId}0/last-logins?equipmentTypeId={equipmentTypeId}</t>
-  </si>
-  <si>
-    <t>/activity/v1/users/{userId}/last-logins?equipmentTypeId={equipmentTypeId}0</t>
-  </si>
-  <si>
     <t>Get User Activity with startTimeStamp and endTimeStamp queries</t>
   </si>
   <si>
@@ -280,6 +271,120 @@
   </si>
   <si>
     <t>/activity/v1/users/a416e744-c66f-48b1-af78-055aa30aa982/simultaneous-logins?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>Get user sessions, filter by equipmentId</t>
+  </si>
+  <si>
+    <t>Get user sessions, filter by locationId</t>
+  </si>
+  <si>
+    <t>Get user sessions, filter by equipmentTypeId</t>
+  </si>
+  <si>
+    <t>Get Last login with startTimeStamp and endTimeStamp queries</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/sessions&amp;equipmentTypeId={equipmentTypeId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/sessions&amp;locationId={locationId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/sessions&amp;equipmentId={equipmentId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/a416e744-c66f-48b1-af78-055aa30aa982/sessions&amp;equipmentId={equipmentId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/sessions&amp;equipmentId=a416e744-c66f-48b1-af78-055aa30aa982</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/sessions?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>Get Simultaneous User Activty without startTimeStamp &amp; endTimeStamp</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous</t>
+  </si>
+  <si>
+    <t>Get Simultaneous User Activity, filter by locationId</t>
+  </si>
+  <si>
+    <t>Get Simultaneous User Activity with pageSize=1</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous?pageSize=1</t>
+  </si>
+  <si>
+    <t>Get Simultaneous User Activty without startTimeStamp</t>
+  </si>
+  <si>
+    <t>Get Simultaneous User Activty without endTimeStamp</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous?endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous?startTimestamp=2020-5-1</t>
+  </si>
+  <si>
+    <t>Get Simultaneous User Activity, filter by invalid locationId</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1?locationId={locationId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1?locationId=123456</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous-logins?endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous-logins?startTimestamp=2020-5-1</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous-logins</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous-logins?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1&amp;pageSize=1</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous-logins?locationId={locationId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous-logins?locationId=a416e744-c66f-48b1-af78-055aa30aa982</t>
+  </si>
+  <si>
+    <t>Get User Summary, filter by locationId</t>
+  </si>
+  <si>
+    <t>Get User Summary with startTimeStamp and endTimeStamp queries</t>
+  </si>
+  <si>
+    <t>Get user Summary, filter by equipmentId</t>
+  </si>
+  <si>
+    <t>Get user Summary, filter by equipmentTypeId</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/summary?locationId={locationId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/summary?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/summary?equipmentTypeId={equipmentTypeId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/last-logins?equipmentTypeId={equipmentId}0</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}0/last-logins?equipmentTypeId={equipmentId}</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/summary?equipmentId={equipmentId}</t>
   </si>
 </sst>
 </file>
@@ -334,7 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -346,6 +451,18 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -668,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7E84D1-294A-4626-81FA-9856648E2C09}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -678,9 +795,9 @@
     <col min="3" max="3" width="45" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.54296875" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="50.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="92.54296875" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.36328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.26953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6328125" style="1" customWidth="1"/>
     <col min="9" max="9" width="19.90625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.7265625" style="1"/>
   </cols>
@@ -734,7 +851,7 @@
         <v>8</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -803,7 +920,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>29</v>
@@ -829,85 +946,85 @@
         <v>8</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -921,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B88D30-C8DE-42A0-A9E2-8B6287FAD006}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -930,7 +1047,7 @@
     <col min="3" max="3" width="55.90625" customWidth="1"/>
     <col min="4" max="4" width="43.90625" customWidth="1"/>
     <col min="6" max="6" width="68.1796875" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" customWidth="1"/>
     <col min="8" max="8" width="25.81640625" customWidth="1"/>
     <col min="9" max="9" width="26.1796875" customWidth="1"/>
   </cols>
@@ -983,15 +1100,13 @@
       <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>39</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
@@ -1010,7 +1125,7 @@
       <c r="F3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="10" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1026,22 +1141,22 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -1053,22 +1168,22 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5">
+        <v>66</v>
+      </c>
+      <c r="G5" s="11">
         <v>200</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1079,22 +1194,22 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6">
+        <v>67</v>
+      </c>
+      <c r="G6" s="11">
         <v>200</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1105,18 +1220,18 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7">
+        <v>113</v>
+      </c>
+      <c r="G7" s="11">
         <v>400</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -1131,18 +1246,18 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8">
+        <v>112</v>
+      </c>
+      <c r="G8" s="11">
         <v>400</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -1157,7 +1272,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>14</v>
@@ -1166,13 +1281,13 @@
         <v>5</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9">
+        <v>69</v>
+      </c>
+      <c r="G9" s="11">
         <v>200</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1192,13 +1307,13 @@
         <v>5</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10">
+        <v>70</v>
+      </c>
+      <c r="G10" s="11">
         <v>200</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1218,10 +1333,13 @@
         <v>5</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11">
+        <v>71</v>
+      </c>
+      <c r="G11" s="11">
         <v>200</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1232,18 +1350,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3388F2-1909-45A3-81C6-E34A543E1DC2}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="3" max="3" width="59.36328125" customWidth="1"/>
     <col min="4" max="4" width="43.90625" customWidth="1"/>
-    <col min="6" max="6" width="52.6328125" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="6" max="6" width="70.26953125" customWidth="1"/>
+    <col min="7" max="7" width="22" style="11" customWidth="1"/>
     <col min="8" max="8" width="25.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1266,7 +1384,7 @@
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -1292,11 +1410,11 @@
       <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1307,16 +1425,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1324,22 +1442,160 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="11">
+        <v>200</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="11">
+        <v>200</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="11">
+        <v>400</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="11">
+        <v>400</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="11">
+        <v>200</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1349,19 +1605,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1505332-9685-449B-8C4A-AB02E3790084}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="42.26953125" customWidth="1"/>
-    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="3" max="3" width="62.90625" customWidth="1"/>
+    <col min="4" max="4" width="43.90625" customWidth="1"/>
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
     <col min="6" max="6" width="67.08984375" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" style="11" customWidth="1"/>
     <col min="8" max="8" width="33.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1384,7 +1640,7 @@
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -1410,15 +1666,15 @@
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1427,17 +1683,175 @@
       <c r="C3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="10" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="11">
+        <v>200</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" s="11">
+        <v>400</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="11">
+        <v>400</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1448,16 +1862,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C3772B-6738-4612-BB2C-6B6DC76D6E13}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="30.1796875" customWidth="1"/>
-    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="3" max="3" width="62.81640625" customWidth="1"/>
+    <col min="4" max="4" width="50.453125" customWidth="1"/>
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
     <col min="6" max="6" width="82.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
@@ -1514,7 +1928,7 @@
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1525,18 +1939,174 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="G3">
         <v>400</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4">
+        <v>400</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>400</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6">
+        <v>400</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7">
+        <v>200</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9">
+        <v>400</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1547,18 +2117,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086B76B2-2B82-421F-92E2-E6E040E4DE28}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="36.453125" customWidth="1"/>
-    <col min="4" max="4" width="43.90625" customWidth="1"/>
-    <col min="6" max="6" width="36.08984375" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="3" max="3" width="59.36328125" customWidth="1"/>
+    <col min="4" max="4" width="49.81640625" customWidth="1"/>
+    <col min="6" max="6" width="69.54296875" customWidth="1"/>
+    <col min="7" max="7" width="19.6328125" style="11" customWidth="1"/>
     <col min="8" max="8" width="25.81640625" customWidth="1"/>
     <col min="9" max="9" width="26.1796875" customWidth="1"/>
   </cols>
@@ -1582,7 +2152,7 @@
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -1608,11 +2178,11 @@
       <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1623,16 +2193,18 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1640,22 +2212,98 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="11">
+        <v>200</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="11">
+        <v>200</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="11">
+        <v>200</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added all the tests for the first endpoint of the utilization feature
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity_Productivity.xlsx
+++ b/src/test/resources/data/Activity_Productivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095D566B-BAF7-4323-BFCD-BC43DAB8913E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7A4111-F674-4AF2-A21E-EBA630E3EB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="0" windowWidth="18510" windowHeight="10110" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="117">
   <si>
     <t>TCID</t>
   </si>
@@ -282,9 +282,6 @@
     <t>Get user sessions, filter by equipmentTypeId</t>
   </si>
   <si>
-    <t>Get Last login with startTimeStamp and endTimeStamp queries</t>
-  </si>
-  <si>
     <t>/activity/v1/users/{userId}/sessions&amp;equipmentTypeId={equipmentTypeId}</t>
   </si>
   <si>
@@ -385,6 +382,15 @@
   </si>
   <si>
     <t>/activity/v1/users/{userId}/summary?equipmentId={equipmentId}</t>
+  </si>
+  <si>
+    <t>Get user sessions using invalid userId and valid equipmentId</t>
+  </si>
+  <si>
+    <t>Get user sessions with valid userId and invalid equipmentId</t>
+  </si>
+  <si>
+    <t>Get user sessions with startTimeStamp and endTimeStamp queries</t>
   </si>
 </sst>
 </file>
@@ -785,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7E84D1-294A-4626-81FA-9856648E2C09}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C3:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1039,7 +1045,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1229,7 +1235,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G7" s="11">
         <v>400</v>
@@ -1255,7 +1261,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G8" s="11">
         <v>400</v>
@@ -1352,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3388F2-1909-45A3-81C6-E34A543E1DC2}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1458,7 +1464,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>8</v>
@@ -1484,7 +1490,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G5" s="11">
         <v>200</v>
@@ -1510,7 +1516,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G6" s="11">
         <v>200</v>
@@ -1527,7 +1533,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>72</v>
@@ -1536,7 +1542,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G7" s="11">
         <v>400</v>
@@ -1553,7 +1559,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>72</v>
@@ -1562,7 +1568,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" s="11">
         <v>400</v>
@@ -1579,7 +1585,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>72</v>
@@ -1588,7 +1594,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G9" s="11">
         <v>200</v>
@@ -1707,7 +1713,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
@@ -1716,7 +1722,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>24</v>
@@ -1733,7 +1739,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
@@ -1742,7 +1748,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>24</v>
@@ -1759,7 +1765,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
@@ -1768,7 +1774,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>24</v>
@@ -1785,7 +1791,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>14</v>
@@ -1794,7 +1800,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G7" s="11">
         <v>200</v>
@@ -1811,7 +1817,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>72</v>
@@ -1820,7 +1826,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G8" s="11">
         <v>400</v>
@@ -1837,7 +1843,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>14</v>
@@ -1846,7 +1852,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G9" s="11">
         <v>400</v>
@@ -1962,7 +1968,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
@@ -1971,7 +1977,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G4">
         <v>400</v>
@@ -1988,7 +1994,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
@@ -1997,7 +2003,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G5">
         <v>400</v>
@@ -2014,7 +2020,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
@@ -2023,7 +2029,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G6">
         <v>400</v>
@@ -2040,7 +2046,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>14</v>
@@ -2049,7 +2055,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G7">
         <v>200</v>
@@ -2066,7 +2072,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>72</v>
@@ -2075,7 +2081,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G8">
         <v>200</v>
@@ -2092,7 +2098,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>14</v>
@@ -2101,7 +2107,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G9">
         <v>400</v>
@@ -2219,14 +2225,14 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>8</v>
@@ -2243,14 +2249,14 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G5" s="11">
         <v>200</v>
@@ -2267,13 +2273,13 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>72</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G6" s="11">
         <v>200</v>
@@ -2290,13 +2296,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>72</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" s="11">
         <v>200</v>

</xml_diff>

<commit_message>
finished writing tests for activity service
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity_Productivity.xlsx
+++ b/src/test/resources/data/Activity_Productivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7A4111-F674-4AF2-A21E-EBA630E3EB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FD7887-8390-43D5-93B4-5D004F1BA766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="18285" yWindow="-21465" windowWidth="31605" windowHeight="20340" firstSheet="1" activeTab="5" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="118">
   <si>
     <t>TCID</t>
   </si>
@@ -78,9 +78,6 @@
     <t>/activity/v1/users?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1&amp;pageSize=100</t>
   </si>
   <si>
-    <t>Get Last Login</t>
-  </si>
-  <si>
     <t>/activity/v1/users/{userId}/last-logins</t>
   </si>
   <si>
@@ -312,9 +309,6 @@
     <t>Get Simultaneous User Activity with pageSize=1</t>
   </si>
   <si>
-    <t>/activity/v1/users/{userId}/simultaneous?pageSize=1</t>
-  </si>
-  <si>
     <t>Get Simultaneous User Activty without startTimeStamp</t>
   </si>
   <si>
@@ -330,9 +324,6 @@
     <t>Get Simultaneous User Activity, filter by invalid locationId</t>
   </si>
   <si>
-    <t>/activity/v1/users/{userId}/simultaneous?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1?locationId={locationId}</t>
-  </si>
-  <si>
     <t>/activity/v1/users/{userId}/simultaneous?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1?locationId=123456</t>
   </si>
   <si>
@@ -391,6 +382,18 @@
   </si>
   <si>
     <t>Get user sessions with startTimeStamp and endTimeStamp queries</t>
+  </si>
+  <si>
+    <t>Get Last Login for user</t>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1&amp;pageSize=1</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1&amp;locationId={locationId}</t>
   </si>
 </sst>
 </file>
@@ -831,10 +834,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -857,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -868,19 +871,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -891,19 +894,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -914,22 +917,22 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -940,97 +943,97 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1045,7 +1048,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1081,10 +1084,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -1095,22 +1098,22 @@
         <v>7</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="7"/>
     </row>
@@ -1122,20 +1125,20 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -1147,22 +1150,22 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -1174,22 +1177,22 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" s="11">
         <v>200</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1200,22 +1203,22 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6" s="11">
         <v>200</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1226,22 +1229,22 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G7" s="11">
         <v>400</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1252,22 +1255,22 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G8" s="11">
         <v>400</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1278,22 +1281,22 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="G9" s="11">
         <v>200</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1304,22 +1307,22 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G10" s="11">
         <v>200</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1330,22 +1333,22 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G11" s="11">
         <v>200</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1356,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3388F2-1909-45A3-81C6-E34A543E1DC2}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1394,7 +1397,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1405,22 +1408,22 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1431,20 +1434,20 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1455,23 +1458,21 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
@@ -1481,23 +1482,21 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G5" s="11">
-        <v>200</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>404</v>
+      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
@@ -1507,23 +1506,21 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="G6" s="11">
-        <v>200</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>404</v>
+      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
@@ -1533,22 +1530,22 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G7" s="11">
         <v>400</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1559,23 +1556,21 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G8" s="11">
-        <v>400</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>404</v>
+      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
@@ -1585,22 +1580,27 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G9" s="11">
         <v>200</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1613,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1505332-9685-449B-8C4A-AB02E3790084}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1624,7 +1624,7 @@
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
     <col min="6" max="6" width="67.08984375" customWidth="1"/>
     <col min="7" max="7" width="18.1796875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="33.453125" customWidth="1"/>
+    <col min="8" max="8" width="48.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1650,7 +1650,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1661,22 +1661,22 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1687,22 +1687,22 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1713,22 +1713,22 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="G4" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1739,22 +1739,22 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="G5" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1765,22 +1765,22 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="G6" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1791,22 +1791,22 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="G7" s="11">
         <v>200</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1817,22 +1817,22 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="G8" s="11">
         <v>400</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1843,22 +1843,22 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G9" s="11">
         <v>400</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1908,7 +1908,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1919,22 +1919,22 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1945,19 +1945,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3">
         <v>400</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1968,22 +1968,22 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G4">
         <v>400</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1994,22 +1994,22 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G5">
         <v>400</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -2020,22 +2020,22 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G6">
         <v>400</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -2046,22 +2046,22 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G7">
         <v>200</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -2072,22 +2072,22 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G8">
         <v>200</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -2098,22 +2098,22 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G9">
         <v>400</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2125,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086B76B2-2B82-421F-92E2-E6E040E4DE28}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2162,7 +2162,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -2173,22 +2173,22 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -2199,22 +2199,22 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="G3" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -2225,20 +2225,20 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -2249,20 +2249,20 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G5" s="11">
         <v>200</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -2273,19 +2273,19 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="G6" s="11">
         <v>200</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -2296,19 +2296,19 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G7" s="11">
         <v>200</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>